<commit_message>
Speak recordings sound, listen terrible. Noted.
</commit_message>
<xml_diff>
--- a/SupportingDocs/WIMR_Config_testing.xlsx
+++ b/SupportingDocs/WIMR_Config_testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OG_Repos\Flinders-EEG-pipeline\SupportingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17BE9FC-60D3-44F3-9691-AC9AC6C6E9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7B68F5-3C30-4901-A837-FD0AF5F473C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>